<commit_message>
Updated Naming_convention_example.xlsx switching order of author last names
</commit_message>
<xml_diff>
--- a/metadata/Naming_convention_example.xlsx
+++ b/metadata/Naming_convention_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengx\Documents\CRISPRflow\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karencheng/CRISPRflow/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B152D-7AC5-40BF-B9C5-98C907822A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A1B2FA9-38C9-6E41-A63D-D62EA06694C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="3840" windowWidth="26940" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1580" windowWidth="26940" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_info" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Last name (first author)</t>
   </si>
   <si>
-    <t>Last name (last author)</t>
-  </si>
-  <si>
     <t>(Virus name)-(serotype)-(type e.g. replicon)-(extra)</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>fastq/from_sequencer/S3_L001_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>Last name (Last author)</t>
   </si>
 </sst>
 </file>
@@ -732,117 +732,117 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -863,36 +863,36 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -913,36 +913,36 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -963,36 +963,36 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1013,6 +1013,18 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
     </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1025,68 +1037,68 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="145.5703125" customWidth="1"/>
-    <col min="2" max="2" width="96.5703125" customWidth="1"/>
+    <col min="1" max="1" width="145.5" customWidth="1"/>
+    <col min="2" max="2" width="96.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,Analysis_info!J6,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A6,Analysis_info!B6,Analysis_info!C6,Analysis_info!D6,Analysis_info!E6,Analysis_info!F6,Analysis_info!G6,Analysis_info!H6,Analysis_info!I6))</f>
-        <v>fastq/example-R1/Cheng_Kistler_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R1_.fastq.gz</v>
+        <v>fastq/example-R1/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R1_.fastq.gz</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,Analysis_info!J7,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A7,Analysis_info!B7,Analysis_info!C7,Analysis_info!D7,Analysis_info!E7,Analysis_info!F7,Analysis_info!G7,Analysis_info!H7,Analysis_info!I7))</f>
-        <v>fastq/example-R1/Cheng_Kistler_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R1_.fastq.gz</v>
+        <v>fastq/example-R1/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R1_.fastq.gz</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="str">
         <f>_xlfn.SINGLE(_xlfn.TEXTJOIN("",TRUE,Analysis_info!J8,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A8,Analysis_info!B8,Analysis_info!C8,Analysis_info!D8,Analysis_info!E8,Analysis_info!F8,Analysis_info!G8,Analysis_info!H8,Analysis_info!I8)))</f>
-        <v>fastq/example-R2/Cheng_Kistler_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R2_.fastq.gz</v>
+        <v>fastq/example-R2/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R2_.fastq.gz</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="str">
         <f>_xlfn.SINGLE(_xlfn.TEXTJOIN("",TRUE,Analysis_info!J9,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A9,Analysis_info!B9,Analysis_info!C9,Analysis_info!D9,Analysis_info!E9,Analysis_info!F9,Analysis_info!G9,Analysis_info!H9,Analysis_info!I9)))</f>
-        <v>fastq/example-R2/Cheng_Kistler_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R2_.fastq.gz</v>
+        <v>fastq/example-R2/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R2_.fastq.gz</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a bug in split library mode
</commit_message>
<xml_diff>
--- a/metadata/Naming_convention_example.xlsx
+++ b/metadata/Naming_convention_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karencheng/CRISPRflow/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duo.peng\Documents\CRISPRflow\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A1B2FA9-38C9-6E41-A63D-D62EA06694C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FAB63D-529E-4B58-87D9-9A82B1D72F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1580" windowWidth="26940" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13635" yWindow="-19290" windowWidth="34935" windowHeight="17130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_info" sheetId="1" r:id="rId1"/>
@@ -142,99 +142,6 @@
   </si>
   <si>
     <r>
-      <t>Library Files [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Manually entered</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, please use </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>one line</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>separated by semicolon if using split library files</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>] [Enter the path</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative to the CRISPRflow directory</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Path to sequencer generated fastq.gz files [</t>
     </r>
     <r>
@@ -385,6 +292,143 @@
   </si>
   <si>
     <t>Last name (Last author)</t>
+  </si>
+  <si>
+    <r>
+      <t>Library Files [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Manually entered</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, please use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one line</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>separated by semicolon if using split library files</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>] [Enter the path</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative to the CRISPRflow directory</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>] Note: if using split library, please include "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_splitA_"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">_splitB_" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in the name of your library files (note the flanking underscore) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -498,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -512,6 +556,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -734,53 +781,53 @@
   </sheetPr>
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.5" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>2</v>
@@ -798,7 +845,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>7</v>
@@ -813,7 +860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -863,7 +910,7 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -913,7 +960,7 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -963,7 +1010,7 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1013,16 +1060,16 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
   </sheetData>
@@ -1037,68 +1084,68 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="145.5" customWidth="1"/>
-    <col min="2" max="2" width="96.5" customWidth="1"/>
+    <col min="1" max="1" width="145.42578125" customWidth="1"/>
+    <col min="2" max="2" width="96.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,Analysis_info!J6,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A6,Analysis_info!B6,Analysis_info!C6,Analysis_info!D6,Analysis_info!E6,Analysis_info!F6,Analysis_info!G6,Analysis_info!H6,Analysis_info!I6))</f>
         <v>fastq/example-R1/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R1_.fastq.gz</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,Analysis_info!J7,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A7,Analysis_info!B7,Analysis_info!C7,Analysis_info!D7,Analysis_info!E7,Analysis_info!F7,Analysis_info!G7,Analysis_info!H7,Analysis_info!I7))</f>
         <v>fastq/example-R1/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R1_.fastq.gz</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
         <f>_xlfn.SINGLE(_xlfn.TEXTJOIN("",TRUE,Analysis_info!J8,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A8,Analysis_info!B8,Analysis_info!C8,Analysis_info!D8,Analysis_info!E8,Analysis_info!F8,Analysis_info!G8,Analysis_info!H8,Analysis_info!I8)))</f>
         <v>fastq/example-R2/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_unsorted_Brunello_Full_R2_.fastq.gz</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
         <f>_xlfn.SINGLE(_xlfn.TEXTJOIN("",TRUE,Analysis_info!J9,"/",_xlfn.TEXTJOIN("_",TRUE,Analysis_info!A9,Analysis_info!B9,Analysis_info!C9,Analysis_info!D9,Analysis_info!E9,Analysis_info!F9,Analysis_info!G9,Analysis_info!H9,Analysis_info!I9)))</f>
         <v>fastq/example-R2/Kistler_Cheng_DENV-2-replicon_Huh751-Cas9-Hygro_low_Brunello_Full_R2_.fastq.gz</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>